<commit_message>
- Caso de uso manter pacientes - Caso de uso Avaliacoes - Atualizacao do documento de ESPECIFICACAO_DE_REQUISITOS_V1.0_CARLOSH.doc - Autalizacao do Documento de Riscos do Projeto.xlsx
</commit_message>
<xml_diff>
--- a/Documentos/4 - Planejamento e Monitoria/Documento de Riscos do Projeto.xlsx
+++ b/Documentos/4 - Planejamento e Monitoria/Documento de Riscos do Projeto.xlsx
@@ -431,7 +431,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9:D10"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -599,10 +599,10 @@
         <v>13</v>
       </c>
       <c r="C9" s="6">
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:14">

</xml_diff>